<commit_message>
The part of EIGRP it's practically finished, confirmation is missing to finish DHCP and do all of 'Sucursal 2'.
</commit_message>
<xml_diff>
--- a/Address tables.xlsx
+++ b/Address tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gfran\Documents\CCNA-Basic-business-network-setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D5C301-1C53-4C3C-A61B-6AC41F713803}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACF4491-E31E-435F-82F1-289EE403CECC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7995" xr2:uid="{C914355B-87B5-4A96-8539-0F26E9395576}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="71">
   <si>
     <t>Equipamento</t>
   </si>
@@ -203,9 +203,6 @@
     <t>192.168.10.118</t>
   </si>
   <si>
-    <t>192.168.10.48/112</t>
-  </si>
-  <si>
     <t>192.168.10.128/27</t>
   </si>
   <si>
@@ -246,6 +243,12 @@
   </si>
   <si>
     <t>Sucursal 1</t>
+  </si>
+  <si>
+    <t>192.168.10.112/29</t>
+  </si>
+  <si>
+    <t>10.0.0.2</t>
   </si>
 </sst>
 </file>
@@ -343,14 +346,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -359,6 +359,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -674,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9143F556-FB84-4667-8E2D-AEA8054DC24B}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,31 +726,31 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" s="5">
+        <v>61</v>
+      </c>
+      <c r="D2" s="3">
         <v>255255255224</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="A3" s="7"/>
       <c r="B3" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="3">
         <v>255255255224</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -755,14 +758,14 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="3">
         <v>255255255240</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -782,14 +785,14 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <v>255255255248</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -797,29 +800,27 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="3">
+        <v>255255255252</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D6" s="5">
-        <v>255255255224</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="5">
+      <c r="C7" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="3">
         <v>255255255224</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -827,16 +828,14 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>69</v>
-      </c>
+      <c r="A8" s="8"/>
       <c r="B8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="5">
+        <v>65</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="3">
         <v>255255255224</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -844,71 +843,88 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
+      <c r="A9" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="5">
-        <v>255255255240</v>
+        <v>51</v>
+      </c>
+      <c r="D9" s="3">
+        <v>255255255224</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
+      <c r="A10" s="5"/>
       <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="5">
-        <v>255255255248</v>
+        <v>53</v>
+      </c>
+      <c r="D10" s="3">
+        <v>255255255240</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
+      <c r="A11" s="5"/>
       <c r="B11" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" s="5">
-        <v>255255255224</v>
+        <v>28</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="3">
+        <v>255255255248</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="3">
+        <v>255255255224</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>31</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>30</v>
       </c>
-      <c r="C15" t="s">
-        <v>63</v>
-      </c>
-      <c r="D15" s="2">
+      <c r="C16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="2">
         <v>255255255224</v>
       </c>
-      <c r="E15" t="s">
-        <v>62</v>
+      <c r="E16" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A2:A8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -920,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{418EEBD5-541B-4B78-A99C-BEDB650C8F20}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,13 +949,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1010,13 +1026,13 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -1077,7 +1093,7 @@
         <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>54</v>
@@ -1087,13 +1103,13 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1120,10 +1136,10 @@
         <v>14</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>20</v>
@@ -1137,10 +1153,10 @@
         <v>15</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>21</v>
@@ -1154,10 +1170,10 @@
         <v>16</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Finish the routing part, eigrp and internet connection.
</commit_message>
<xml_diff>
--- a/Address tables.xlsx
+++ b/Address tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gfran\Documents\CCNA-Basic-business-network-setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACF4491-E31E-435F-82F1-289EE403CECC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F4F86B-DB92-45FD-BDCA-947ED95C93BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7995" xr2:uid="{C914355B-87B5-4A96-8539-0F26E9395576}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{C914355B-87B5-4A96-8539-0F26E9395576}"/>
   </bookViews>
   <sheets>
     <sheet name="Equipamentos" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="73">
   <si>
     <t>Equipamento</t>
   </si>
@@ -239,9 +239,6 @@
     <t>192.168.10.226</t>
   </si>
   <si>
-    <t>192.168.10.227</t>
-  </si>
-  <si>
     <t>Sucursal 1</t>
   </si>
   <si>
@@ -249,6 +246,15 @@
   </si>
   <si>
     <t>10.0.0.2</t>
+  </si>
+  <si>
+    <t>Sucursal 2</t>
+  </si>
+  <si>
+    <t>192.168.10.229</t>
+  </si>
+  <si>
+    <t>192.168.10.230</t>
   </si>
 </sst>
 </file>
@@ -342,7 +348,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -363,6 +369,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9143F556-FB84-4667-8E2D-AEA8054DC24B}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,7 +812,7 @@
         <v>64</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D6" s="3">
         <v>255255255252</v>
@@ -821,7 +828,7 @@
         <v>63</v>
       </c>
       <c r="D7" s="3">
-        <v>255255255224</v>
+        <v>255255255252</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>27</v>
@@ -833,10 +840,10 @@
         <v>65</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D8" s="3">
-        <v>255255255224</v>
+        <v>255255255252</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>27</v>
@@ -844,7 +851,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>24</v>
@@ -873,6 +880,7 @@
       <c r="E10" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
@@ -895,36 +903,99 @@
         <v>64</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D12" s="3">
-        <v>255255255224</v>
+        <v>255255255252</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>27</v>
       </c>
     </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="3">
+        <v>255255255224</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="3">
+        <v>255255255240</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="3">
+        <v>255255255248</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="5"/>
+      <c r="B16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="3">
+        <v>255255255252</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>31</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B21" t="s">
         <v>30</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C21" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D21" s="2">
         <v>255255255224</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E21" t="s">
         <v>61</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A13:A16"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -936,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{418EEBD5-541B-4B78-A99C-BEDB650C8F20}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,7 +1164,7 @@
         <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>54</v>
@@ -1194,7 +1265,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E4" sqref="A1:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,70 +1278,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
The VPN part and ISP connection by PPoE have yet to be terminated.
</commit_message>
<xml_diff>
--- a/Address tables.xlsx
+++ b/Address tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gfran\Documents\CCNA-Basic-business-network-setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F4F86B-DB92-45FD-BDCA-947ED95C93BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D7BFB9-4D17-4E8B-BCE3-83A46EC3313B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{C914355B-87B5-4A96-8539-0F26E9395576}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="91">
   <si>
     <t>Equipamento</t>
   </si>
@@ -53,18 +53,6 @@
     <t>Default Gateway</t>
   </si>
   <si>
-    <t>1100 0000</t>
-  </si>
-  <si>
-    <t>1010 1000</t>
-  </si>
-  <si>
-    <t>0000 1010</t>
-  </si>
-  <si>
-    <t>0000 0000</t>
-  </si>
-  <si>
     <t>VLAN ID</t>
   </si>
   <si>
@@ -89,15 +77,6 @@
     <t>Administracao</t>
   </si>
   <si>
-    <t>192.168.0.254</t>
-  </si>
-  <si>
-    <t>192.168.1.254</t>
-  </si>
-  <si>
-    <t>192.168.2.254</t>
-  </si>
-  <si>
     <t>fa0/2</t>
   </si>
   <si>
@@ -110,33 +89,9 @@
     <t>Sede</t>
   </si>
   <si>
-    <t>FastEthernet 0/1.10</t>
-  </si>
-  <si>
-    <t>192.168.0.1</t>
-  </si>
-  <si>
-    <t>255.255.255.0</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>FastEthernet 0/1.30</t>
-  </si>
-  <si>
-    <t>FastEthernet 0/1.20</t>
-  </si>
-  <si>
-    <t>FastEthernet 0/0</t>
-  </si>
-  <si>
     <t>Main-Server</t>
   </si>
   <si>
-    <t>192.168.10.2</t>
-  </si>
-  <si>
     <t>Pool</t>
   </si>
   <si>
@@ -152,12 +107,6 @@
     <t>Mascara</t>
   </si>
   <si>
-    <t>192.168.1.1</t>
-  </si>
-  <si>
-    <t>192.168.2.1</t>
-  </si>
-  <si>
     <t>192.168.10.0/27</t>
   </si>
   <si>
@@ -176,9 +125,6 @@
     <t>192.168.10.54</t>
   </si>
   <si>
-    <t>Serial 0/1/0</t>
-  </si>
-  <si>
     <t>VLAN Sede</t>
   </si>
   <si>
@@ -230,12 +176,6 @@
     <t>192.168.10.225</t>
   </si>
   <si>
-    <t>Serial 0/0/0</t>
-  </si>
-  <si>
-    <t>Serial 0/1/1</t>
-  </si>
-  <si>
     <t>192.168.10.226</t>
   </si>
   <si>
@@ -255,6 +195,120 @@
   </si>
   <si>
     <t>192.168.10.230</t>
+  </si>
+  <si>
+    <t>Vendas - Sede</t>
+  </si>
+  <si>
+    <t>Recursos Humanos - Sede</t>
+  </si>
+  <si>
+    <t>Administracao - Sede</t>
+  </si>
+  <si>
+    <t>10.0.1.2</t>
+  </si>
+  <si>
+    <t>192.168.10.33</t>
+  </si>
+  <si>
+    <t>192.168.10.49</t>
+  </si>
+  <si>
+    <t>192.168.10.1</t>
+  </si>
+  <si>
+    <t>192.168.10.65</t>
+  </si>
+  <si>
+    <t>192.168.10.97</t>
+  </si>
+  <si>
+    <t>192.168.10.113</t>
+  </si>
+  <si>
+    <t>192.168.10.177</t>
+  </si>
+  <si>
+    <t>192.168.10.161</t>
+  </si>
+  <si>
+    <t>192.168.10.129</t>
+  </si>
+  <si>
+    <t>VendasSede</t>
+  </si>
+  <si>
+    <t>Recursos HumanosSede</t>
+  </si>
+  <si>
+    <t>AdministracaoSede</t>
+  </si>
+  <si>
+    <t>VendasS1</t>
+  </si>
+  <si>
+    <t>Recursos HumanosS1</t>
+  </si>
+  <si>
+    <t>AdministracaoS1</t>
+  </si>
+  <si>
+    <t>VendasS2</t>
+  </si>
+  <si>
+    <t>Recursos HumanosS2</t>
+  </si>
+  <si>
+    <t>AdministracaoS2</t>
+  </si>
+  <si>
+    <t>DHCP</t>
+  </si>
+  <si>
+    <t>Vendas - S1</t>
+  </si>
+  <si>
+    <t>Recursos Humanos - S1</t>
+  </si>
+  <si>
+    <t>Administracao - S1</t>
+  </si>
+  <si>
+    <t>Vendas - S2</t>
+  </si>
+  <si>
+    <t>Recursos Humanos - S2</t>
+  </si>
+  <si>
+    <t>Administracao - S3</t>
+  </si>
+  <si>
+    <t>NIC</t>
+  </si>
+  <si>
+    <t>Não definido.</t>
+  </si>
+  <si>
+    <t>Fa 0/0</t>
+  </si>
+  <si>
+    <t>Fa 0/1.10</t>
+  </si>
+  <si>
+    <t>Fa 0/1.20</t>
+  </si>
+  <si>
+    <t>Fa 0/1.30</t>
+  </si>
+  <si>
+    <t>S 0/0/0</t>
+  </si>
+  <si>
+    <t>S 0/1/0</t>
+  </si>
+  <si>
+    <t>S 0/1/1</t>
   </si>
 </sst>
 </file>
@@ -348,12 +402,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -369,7 +425,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,318 +754,429 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9143F556-FB84-4667-8E2D-AEA8054DC24B}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="H8" activeCellId="1" sqref="E9:E12 H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5703125" customWidth="1"/>
     <col min="9" max="9" width="10.28515625" customWidth="1"/>
     <col min="10" max="10" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1">
-        <v>192</v>
-      </c>
-      <c r="H1">
-        <v>168</v>
-      </c>
-      <c r="I1">
-        <v>10</v>
-      </c>
-      <c r="J1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" s="3">
+        <v>16</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="11">
         <v>255255255224</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E2" s="12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="3">
+      <c r="D3" s="11">
         <v>255255255224</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E3" s="13"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
-      <c r="B4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="11">
+        <v>255255255240</v>
+      </c>
+      <c r="E4" s="13"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="11">
+        <v>255255255248</v>
+      </c>
+      <c r="E5" s="13"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="11">
+        <v>255255255252</v>
+      </c>
+      <c r="E6" s="13"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="11">
+        <v>255255255252</v>
+      </c>
+      <c r="E7" s="13"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="11">
+        <v>255255255252</v>
+      </c>
+      <c r="E8" s="14"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="11">
+        <v>255255255224</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="11">
+        <v>255255255240</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="11">
+        <v>255255255248</v>
+      </c>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="11">
+        <v>255255255252</v>
+      </c>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="11">
+        <v>255255255224</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="11">
+        <v>255255255240</v>
+      </c>
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="11">
+        <v>255255255248</v>
+      </c>
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="11">
+        <v>255255255252</v>
+      </c>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="11">
+        <v>255255255224</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="3">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="11">
+        <v>255255255224</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" s="11">
         <v>255255255240</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="1" t="s">
+      <c r="E19" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="11">
+        <v>255255255248</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="3">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="11">
+        <v>255255255224</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="11">
+        <v>255255255240</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" s="11">
         <v>255255255248</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D6" s="3">
-        <v>255255255252</v>
-      </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="3">
-        <v>255255255252</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" s="3">
-        <v>255255255252</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="3">
+      <c r="E23" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" s="11">
         <v>255255255224</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="3">
+      <c r="E24" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" s="11">
         <v>255255255240</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I10" s="10"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" s="3">
+      <c r="E25" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="11">
         <v>255255255248</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" s="3">
-        <v>255255255252</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="3">
-        <v>255255255224</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" s="3">
-        <v>255255255240</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="3">
-        <v>255255255248</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D16" s="3">
-        <v>255255255252</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="2">
-        <v>255255255224</v>
-      </c>
-      <c r="E21" t="s">
-        <v>61</v>
+      <c r="E26" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="A13:A16"/>
+    <mergeCell ref="E2:E8"/>
+    <mergeCell ref="E9:E12"/>
+    <mergeCell ref="E13:E16"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1007,8 +1188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{418EEBD5-541B-4B78-A99C-BEDB650C8F20}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,7 +1202,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -1030,19 +1211,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1050,16 +1231,16 @@
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1067,16 +1248,16 @@
         <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1084,21 +1265,21 @@
         <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -1107,19 +1288,19 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1127,16 +1308,16 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1144,16 +1325,16 @@
         <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1161,21 +1342,21 @@
         <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -1184,19 +1365,19 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1204,16 +1385,16 @@
         <v>10</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1221,16 +1402,16 @@
         <v>20</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1238,16 +1419,16 @@
         <v>30</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1262,87 +1443,189 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01020C27-4629-4A4D-9AD7-9B77F0CD71F6}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="A1:E4"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" customWidth="1"/>
     <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>26</v>
+        <v>59</v>
+      </c>
+      <c r="E2" s="11">
+        <v>255255255224</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>26</v>
+        <v>57</v>
+      </c>
+      <c r="E3" s="11">
+        <v>255255255240</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>26</v>
+        <v>58</v>
+      </c>
+      <c r="E4" s="11">
+        <v>255255255248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="11">
+        <v>255255255224</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="11">
+        <v>255255255240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="11">
+        <v>255255255248</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="11">
+        <v>255255255224</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="11">
+        <v>255255255240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="11">
+        <v>255255255248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Need finish the VPN and PPPoE part!
</commit_message>
<xml_diff>
--- a/Address tables.xlsx
+++ b/Address tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gfran\Documents\CCNA-Basic-business-network-setup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\CCNA-Basic-business-network-setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C503E0D8-CCA3-40D6-82E2-6C36957050D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9594980A-BF4C-4A06-9F65-6915F267F14C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{C914355B-87B5-4A96-8539-0F26E9395576}"/>
+    <workbookView xWindow="18075" yWindow="2175" windowWidth="9990" windowHeight="11505" xr2:uid="{C914355B-87B5-4A96-8539-0F26E9395576}"/>
   </bookViews>
   <sheets>
     <sheet name="Equipamentos" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="101">
   <si>
     <t>Equipamento</t>
   </si>
@@ -318,6 +318,27 @@
   </si>
   <si>
     <t>192.168.10.234</t>
+  </si>
+  <si>
+    <t>Empressa Frutas PT</t>
+  </si>
+  <si>
+    <t>Ligação residencial</t>
+  </si>
+  <si>
+    <t>255.255.255.0</t>
+  </si>
+  <si>
+    <t>10.0.0.6</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>192.168.1.1</t>
+  </si>
+  <si>
+    <t>192.168.1.2</t>
   </si>
 </sst>
 </file>
@@ -411,14 +432,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -426,6 +446,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -448,6 +471,28 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -763,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9143F556-FB84-4667-8E2D-AEA8054DC24B}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,300 +822,426 @@
     <col min="4" max="4" width="21" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" customWidth="1"/>
+    <col min="8" max="8" width="24.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="11" max="11" width="21.5703125" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="H1" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="H2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D3" s="6">
         <v>255255255224</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E3" s="11" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="7">
-        <v>255255255224</v>
-      </c>
-      <c r="E3" s="12"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H3" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="7">
-        <v>255255255240</v>
+        <v>24</v>
+      </c>
+      <c r="D4" s="6">
+        <v>255255255224</v>
       </c>
       <c r="E4" s="12"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H4" s="10"/>
+      <c r="I4" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="K4" s="6">
+        <v>255255255252</v>
+      </c>
+      <c r="L4" s="13"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="7">
-        <v>255255255248</v>
+        <v>26</v>
+      </c>
+      <c r="D5" s="6">
+        <v>255255255240</v>
       </c>
       <c r="E5" s="12"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G5" s="2"/>
+      <c r="H5" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="7">
-        <v>255255255252</v>
+        <v>28</v>
+      </c>
+      <c r="D6" s="6">
+        <v>255255255248</v>
       </c>
       <c r="E6" s="12"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H6" s="21"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="22"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="6">
+        <v>255255255252</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="22"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D8" s="6">
         <v>255255255252</v>
       </c>
-      <c r="E7" s="12"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="3" t="s">
+      <c r="E8" s="12"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="22"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D9" s="6">
         <v>255255255252</v>
       </c>
-      <c r="E8" s="13"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="E9" s="13"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="22"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D10" s="6">
         <v>255255255224</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E10" s="8" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="7">
-        <v>255255255240</v>
-      </c>
-      <c r="E10" s="9"/>
-      <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="7">
-        <v>255255255248</v>
+        <v>35</v>
+      </c>
+      <c r="D11" s="6">
+        <v>255255255240</v>
       </c>
       <c r="E11" s="9"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H11" s="15"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="15"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="6">
+        <v>255255255248</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="15"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D13" s="6">
         <v>255255255252</v>
       </c>
-      <c r="E12" s="9"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="5" t="s">
+      <c r="E13" s="9"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="15"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D14" s="6">
         <v>25525552555252</v>
       </c>
-      <c r="E13" s="10"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="E14" s="10"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="15"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D15" s="6">
         <v>255255255224</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E15" s="8" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="7">
-        <v>255255255240</v>
-      </c>
-      <c r="E15" s="9"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H15" s="19"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="19"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="B16" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="7">
-        <v>255255255248</v>
+        <v>40</v>
+      </c>
+      <c r="D16" s="6">
+        <v>255255255240</v>
       </c>
       <c r="E16" s="9"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H16" s="19"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="19"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="6">
+        <v>255255255248</v>
+      </c>
+      <c r="E17" s="9"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="19"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="B18" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D18" s="6">
         <v>255255255252</v>
       </c>
-      <c r="E17" s="9"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="5" t="s">
+      <c r="E18" s="9"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="19"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D19" s="6">
         <v>255255255252</v>
       </c>
-      <c r="E18" s="10"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="E19" s="10"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="19"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="7">
-        <v>255255255224</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>82</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D20" s="7">
+        <v>44</v>
+      </c>
+      <c r="D20" s="6">
         <v>255255255224</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="16"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>82</v>
@@ -1078,16 +1249,21 @@
       <c r="C21" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D21" s="7">
-        <v>255255255240</v>
+      <c r="D21" s="6">
+        <v>255255255224</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>82</v>
@@ -1095,16 +1271,21 @@
       <c r="C22" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D22" s="7">
-        <v>255255255248</v>
+      <c r="D22" s="6">
+        <v>255255255240</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="16"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>82</v>
@@ -1112,16 +1293,21 @@
       <c r="C23" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D23" s="7">
-        <v>255255255224</v>
+      <c r="D23" s="6">
+        <v>255255255248</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="16"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>82</v>
@@ -1129,16 +1315,21 @@
       <c r="C24" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D24" s="7">
-        <v>255255255240</v>
+      <c r="D24" s="6">
+        <v>255255255224</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="16"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>82</v>
@@ -1146,16 +1337,21 @@
       <c r="C25" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D25" s="7">
-        <v>255255255248</v>
+      <c r="D25" s="6">
+        <v>255255255240</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="16"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>82</v>
@@ -1163,16 +1359,21 @@
       <c r="C26" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D26" s="7">
-        <v>255255255224</v>
+      <c r="D26" s="6">
+        <v>255255255248</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="16"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>82</v>
@@ -1180,16 +1381,21 @@
       <c r="C27" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D27" s="7">
-        <v>255255255240</v>
+      <c r="D27" s="6">
+        <v>255255255224</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="16"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>82</v>
@@ -1197,21 +1403,54 @@
       <c r="C28" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="6">
+        <v>255255255240</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="17"/>
+      <c r="L28" s="16"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29" s="6">
         <v>255255255248</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E29" s="3" t="s">
         <v>42</v>
       </c>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="E2:E8"/>
-    <mergeCell ref="A9:A13"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="E14:E18"/>
-    <mergeCell ref="E9:E13"/>
+  <mergeCells count="12">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="H15:H19"/>
+    <mergeCell ref="L15:L19"/>
+    <mergeCell ref="A3:A9"/>
+    <mergeCell ref="E3:E9"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="E15:E19"/>
+    <mergeCell ref="E10:E14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1523,7 +1762,7 @@
       <c r="D2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="6">
         <v>255255255224</v>
       </c>
     </row>
@@ -1540,7 +1779,7 @@
       <c r="D3" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <v>255255255240</v>
       </c>
     </row>
@@ -1557,7 +1796,7 @@
       <c r="D4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="6">
         <v>255255255248</v>
       </c>
     </row>
@@ -1574,7 +1813,7 @@
       <c r="D5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="6">
         <v>255255255224</v>
       </c>
     </row>
@@ -1591,7 +1830,7 @@
       <c r="D6" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>255255255240</v>
       </c>
     </row>
@@ -1608,7 +1847,7 @@
       <c r="D7" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>255255255248</v>
       </c>
     </row>
@@ -1625,7 +1864,7 @@
       <c r="D8" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <v>255255255224</v>
       </c>
     </row>
@@ -1642,7 +1881,7 @@
       <c r="D9" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <v>255255255240</v>
       </c>
     </row>
@@ -1659,7 +1898,7 @@
       <c r="D10" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="6">
         <v>255255255248</v>
       </c>
     </row>

</xml_diff>